<commit_message>
modifying variable names in data engineering
</commit_message>
<xml_diff>
--- a/data_engineering/BDD_for_dataviz.xlsx
+++ b/data_engineering/BDD_for_dataviz.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>c1_1_8deg_final</t>
+          <t>c1_1_8_deg_final</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -456,7 +456,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>C1_final_date</t>
+          <t>c1_final_date</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -466,27 +466,27 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>C1_initial_date</t>
+          <t>c1_initial_date</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>c2_1_5deg_final</t>
+          <t>c2_1_5_deg_final</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>c2_1_8deg_final</t>
+          <t>c2_1_8_deg_final</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>c2_2deg_final</t>
+          <t>c2_2_deg_final</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>C2_final_date</t>
+          <t>c2_final_date</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>C2_initial_date</t>
+          <t>c2_initial_date</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">

</xml_diff>